<commit_message>
soft delete added & phone number validation added
</commit_message>
<xml_diff>
--- a/downloads/userdata.xlsx
+++ b/downloads/userdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhyan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECT\nova\server-side\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5234165-BAD5-4870-9C65-3C20D92DCFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7B9972-8A75-4046-A15C-E41F8D88552B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,7 +348,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,7 +383,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5555555555</v>
+        <v>55555555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data insert from xml file
</commit_message>
<xml_diff>
--- a/downloads/userdata.xlsx
+++ b/downloads/userdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECT\nova\server-side\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7B9972-8A75-4046-A15C-E41F8D88552B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3EB0EF-8A3B-4D50-AD0D-1FAA55AD9DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>(726) 222 - 1745</t>
   </si>
 </sst>
 </file>
@@ -345,15 +348,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -386,6 +389,11 @@
         <v>55555555555</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>